<commit_message>
INotifyPropertyChanged and Command arg
</commit_message>
<xml_diff>
--- a/PI-TECH-TEST.xlsx
+++ b/PI-TECH-TEST.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11595" windowHeight="7665"/>
+    <workbookView windowWidth="19815" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
   <si>
     <t>SUBJECT</t>
   </si>
   <si>
-    <t>MS SQL SERVER</t>
+    <t xml:space="preserve">C# </t>
   </si>
   <si>
     <t>NAME</t>
@@ -37,16 +37,25 @@
     <t>ANS</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
-    <t>B</t>
+    <t>IEnumerable&lt;Employee&gt; query1 = from emp in empList where emp.deptname="HR" and emp.salary&gt;25000 and  select emp;</t>
+  </si>
+  <si>
+    <t>IEnumerable&lt;Employee&gt; query2=empList.where(emp=&gt;emp.deptname="HR", emp=&gt;emp.salary&gt;25000)</t>
+  </si>
+  <si>
+    <t>connectionString="Server= VSTS2017/SQLExpress; Database=Training;User ID=admin;Password=admin@123;"</t>
   </si>
 </sst>
 </file>
@@ -55,10 +64,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -69,6 +78,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -77,15 +107,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -94,21 +118,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -123,17 +132,33 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -161,22 +186,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -184,30 +216,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,13 +231,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,31 +381,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,7 +399,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,121 +411,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,9 +466,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -475,6 +486,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,164 +522,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -667,7 +676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -989,10 +998,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1021,7 +1030,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>44370</v>
+        <v>44383</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1055,13 +1064,13 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G6">
         <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1069,7 +1078,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <v>12</v>
@@ -1081,7 +1090,7 @@
         <v>22</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1089,13 +1098,13 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <v>23</v>
@@ -1109,13 +1118,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9">
         <v>24</v>
@@ -1129,7 +1138,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>15</v>
@@ -1149,19 +1158,19 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G11">
         <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1181,7 +1190,7 @@
         <v>27</v>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1209,19 +1218,19 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G14">
         <v>29</v>
       </c>
       <c r="H14" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1229,7 +1238,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>20</v>
@@ -1237,11 +1246,16 @@
       <c r="E15" t="s">
         <v>7</v>
       </c>
-      <c r="G15">
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8">
+      <c r="G17">
         <v>30</v>
       </c>
-      <c r="H15" t="s">
-        <v>8</v>
+      <c r="H17" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>